<commit_message>
reformat new Rachel neut data and `yaml`
</commit_message>
<xml_diff>
--- a/data/neut_assays/plate_reader_data/VIDD1_NeutralizationAssay.xlsx
+++ b/data/neut_assays/plate_reader_data/VIDD1_NeutralizationAssay.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28109"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juhyemlee/Google Drive/Bloom_Lab/Perth2009_MAP/NeutralizationAssays/mutvalidation/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="30420" yWindow="460" windowWidth="32100" windowHeight="17640"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="WT" sheetId="2" r:id="rId1"/>
@@ -17,14 +12,17 @@
     <sheet name="F193F" sheetId="3" r:id="rId3"/>
     <sheet name="K189D" sheetId="4" r:id="rId4"/>
     <sheet name="L157D" sheetId="5" r:id="rId5"/>
+    <sheet name="WT2" sheetId="6" r:id="rId6"/>
+    <sheet name="F159G" sheetId="7" r:id="rId7"/>
+    <sheet name="K160T" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -475,8 +473,275 @@
 </comments>
 </file>
 
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Eguia, Rachel T</author>
+  </authors>
+  <commentList>
+    <comment ref="E1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.Common, 3.3.10.0
+Tecan.At.Common.DocumentManagement, 3.3.10.0
+Tecan.At.Common.DocumentManagement.Reader, 3.1.17.0
+Tecan.At.Common.MCS, 3.3.10.0
+Tecan.At.Common.Results, 3.3.10.0
+Tecan.At.Common.UI, 3.3.10.0
+Tecan.At.Communication.Common, 3.3.12.0
+Tecan.At.Communication.Port.IP, 3.3.12.0
+Tecan.At.Communication.Port.RS232, 3.3.12.0
+Tecan.At.Communication.Port.SIM.Common, 3.3.12.0
+Tecan.At.Communication.Port.USB, 3.3.12.0
+Tecan.At.Communication.Server, 3.3.12.0
+Tecan.At.Communication.SIM.AMR, 3.1.17.0
+Tecan.At.Communication.SIM.AMRPlus, 3.1.17.0
+Tecan.At.Communication.SIM.Connect, 3.3.12.0
+Tecan.At.Communication.SIM.GeniosUltra, 3.1.17.0
+Tecan.At.Communication.SIM.Safire3, 3.1.17.0
+Tecan.At.Communication.SIM.Safire3Pro, 3.1.17.0
+Tecan.At.Communication.SIM.SunriseMini, 3.1.17.0
+Tecan.At.Instrument.Common, 3.3.12.0
+Tecan.At.Instrument.Common.Reader, 3.1.17.0
+Tecan.At.Instrument.Common.Stacker, 3.3.12.0
+Tecan.At.Instrument.Reader.AMR, 3.1.17.0
+Tecan.At.Instrument.Reader.AMRPlus, 3.1.17.0
+Tecan.At.Instrument.Reader.GeniosUltra, 3.1.17.0
+Tecan.At.Instrument.Reader.Safire3, 3.1.17.0
+Tecan.At.Instrument.Reader.Safire3Pro, 3.1.17.0
+Tecan.At.Instrument.Reader.SunriseMini, 3.1.17.0
+Tecan.At.Instrument.Server, 3.3.12.0
+Tecan.At.Instrument.Stacker.Connect, 3.3.12.0
+Tecan.At.Instrument.Stacker.Server, 3.3.12.0
+Tecan.At.Measurement.BuiltInTest.Common, 3.1.17.0
+Tecan.At.Measurement.Common, 3.1.17.0
+Tecan.At.Measurement.Server, 3.1.17.0
+Tecan.At.XFluor, 1.9.17.0
+Tecan.At.XFluor.Connect.Reader, 1.9.17.0
+Tecan.At.XFluor.Core, 1.9.17.0
+Tecan.At.XFluor.Device, 1.9.17.0
+Tecan.At.XFluor.Device.AMR, 1.9.17.0
+Tecan.At.XFluor.Device.AMRPlus, 1.9.17.0
+Tecan.At.XFluor.Device.GeniosUltra, 1.9.17.0
+Tecan.At.XFluor.Device.Reader, 1.9.17.0
+Tecan.At.XFluor.Device.Safire3, 1.9.17.0
+Tecan.At.XFluor.Device.Safire3Pro, 1.9.17.0
+Tecan.At.XFluor.Device.SunriseMini, 1.9.17.0
+Tecan.At.XFluor.ExcelOutput, 1.9.17.0
+Tecan.At.XFluor.NanoQuant, 1.9.17.0
+Tecan.At.XFluor.ReaderEditor, 1.9.17.0
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">MEX, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
+MEM, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
+ABS, V 1.00 MCR Abs 4 Channel (V 1.00 MCR Abs 4 Channel)
+LUM, V_1.04_11/2011_LUMINESCENCE (Nov 02 2011/17.53.34)
+TCAN, V_1.00_02/2008_S3FTCAN (Feb 21 2008/17.19.16)
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Eguia, Rachel T</author>
+  </authors>
+  <commentList>
+    <comment ref="E1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.Common, 3.3.10.0
+Tecan.At.Common.DocumentManagement, 3.3.10.0
+Tecan.At.Common.DocumentManagement.Reader, 3.1.17.0
+Tecan.At.Common.MCS, 3.3.10.0
+Tecan.At.Common.Results, 3.3.10.0
+Tecan.At.Common.UI, 3.3.10.0
+Tecan.At.Communication.Common, 3.3.12.0
+Tecan.At.Communication.Port.IP, 3.3.12.0
+Tecan.At.Communication.Port.RS232, 3.3.12.0
+Tecan.At.Communication.Port.SIM.Common, 3.3.12.0
+Tecan.At.Communication.Port.USB, 3.3.12.0
+Tecan.At.Communication.Server, 3.3.12.0
+Tecan.At.Communication.SIM.AMR, 3.1.17.0
+Tecan.At.Communication.SIM.AMRPlus, 3.1.17.0
+Tecan.At.Communication.SIM.Connect, 3.3.12.0
+Tecan.At.Communication.SIM.GeniosUltra, 3.1.17.0
+Tecan.At.Communication.SIM.Safire3, 3.1.17.0
+Tecan.At.Communication.SIM.Safire3Pro, 3.1.17.0
+Tecan.At.Communication.SIM.SunriseMini, 3.1.17.0
+Tecan.At.Instrument.Common, 3.3.12.0
+Tecan.At.Instrument.Common.Reader, 3.1.17.0
+Tecan.At.Instrument.Common.Stacker, 3.3.12.0
+Tecan.At.Instrument.Reader.AMR, 3.1.17.0
+Tecan.At.Instrument.Reader.AMRPlus, 3.1.17.0
+Tecan.At.Instrument.Reader.GeniosUltra, 3.1.17.0
+Tecan.At.Instrument.Reader.Safire3, 3.1.17.0
+Tecan.At.Instrument.Reader.Safire3Pro, 3.1.17.0
+Tecan.At.Instrument.Reader.SunriseMini, 3.1.17.0
+Tecan.At.Instrument.Server, 3.3.12.0
+Tecan.At.Instrument.Stacker.Connect, 3.3.12.0
+Tecan.At.Instrument.Stacker.Server, 3.3.12.0
+Tecan.At.Measurement.BuiltInTest.Common, 3.1.17.0
+Tecan.At.Measurement.Common, 3.1.17.0
+Tecan.At.Measurement.Server, 3.1.17.0
+Tecan.At.XFluor, 1.9.17.0
+Tecan.At.XFluor.Connect.Reader, 1.9.17.0
+Tecan.At.XFluor.Core, 1.9.17.0
+Tecan.At.XFluor.Device, 1.9.17.0
+Tecan.At.XFluor.Device.AMR, 1.9.17.0
+Tecan.At.XFluor.Device.AMRPlus, 1.9.17.0
+Tecan.At.XFluor.Device.GeniosUltra, 1.9.17.0
+Tecan.At.XFluor.Device.Reader, 1.9.17.0
+Tecan.At.XFluor.Device.Safire3, 1.9.17.0
+Tecan.At.XFluor.Device.Safire3Pro, 1.9.17.0
+Tecan.At.XFluor.Device.SunriseMini, 1.9.17.0
+Tecan.At.XFluor.ExcelOutput, 1.9.17.0
+Tecan.At.XFluor.NanoQuant, 1.9.17.0
+Tecan.At.XFluor.ReaderEditor, 1.9.17.0
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">MEX, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
+MEM, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
+ABS, V 1.00 MCR Abs 4 Channel (V 1.00 MCR Abs 4 Channel)
+LUM, V_1.04_11/2011_LUMINESCENCE (Nov 02 2011/17.53.34)
+TCAN, V_1.00_02/2008_S3FTCAN (Feb 21 2008/17.19.16)
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Eguia, Rachel T</author>
+  </authors>
+  <commentList>
+    <comment ref="E1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">Tecan.At.Common, 3.3.10.0
+Tecan.At.Common.DocumentManagement, 3.3.10.0
+Tecan.At.Common.DocumentManagement.Reader, 3.1.17.0
+Tecan.At.Common.MCS, 3.3.10.0
+Tecan.At.Common.Results, 3.3.10.0
+Tecan.At.Common.UI, 3.3.10.0
+Tecan.At.Communication.Common, 3.3.12.0
+Tecan.At.Communication.Port.IP, 3.3.12.0
+Tecan.At.Communication.Port.RS232, 3.3.12.0
+Tecan.At.Communication.Port.SIM.Common, 3.3.12.0
+Tecan.At.Communication.Port.USB, 3.3.12.0
+Tecan.At.Communication.Server, 3.3.12.0
+Tecan.At.Communication.SIM.AMR, 3.1.17.0
+Tecan.At.Communication.SIM.AMRPlus, 3.1.17.0
+Tecan.At.Communication.SIM.Connect, 3.3.12.0
+Tecan.At.Communication.SIM.GeniosUltra, 3.1.17.0
+Tecan.At.Communication.SIM.Safire3, 3.1.17.0
+Tecan.At.Communication.SIM.Safire3Pro, 3.1.17.0
+Tecan.At.Communication.SIM.SunriseMini, 3.1.17.0
+Tecan.At.Instrument.Common, 3.3.12.0
+Tecan.At.Instrument.Common.Reader, 3.1.17.0
+Tecan.At.Instrument.Common.Stacker, 3.3.12.0
+Tecan.At.Instrument.Reader.AMR, 3.1.17.0
+Tecan.At.Instrument.Reader.AMRPlus, 3.1.17.0
+Tecan.At.Instrument.Reader.GeniosUltra, 3.1.17.0
+Tecan.At.Instrument.Reader.Safire3, 3.1.17.0
+Tecan.At.Instrument.Reader.Safire3Pro, 3.1.17.0
+Tecan.At.Instrument.Reader.SunriseMini, 3.1.17.0
+Tecan.At.Instrument.Server, 3.3.12.0
+Tecan.At.Instrument.Stacker.Connect, 3.3.12.0
+Tecan.At.Instrument.Stacker.Server, 3.3.12.0
+Tecan.At.Measurement.BuiltInTest.Common, 3.1.17.0
+Tecan.At.Measurement.Common, 3.1.17.0
+Tecan.At.Measurement.Server, 3.1.17.0
+Tecan.At.XFluor, 1.9.17.0
+Tecan.At.XFluor.Connect.Reader, 1.9.17.0
+Tecan.At.XFluor.Core, 1.9.17.0
+Tecan.At.XFluor.Device, 1.9.17.0
+Tecan.At.XFluor.Device.AMR, 1.9.17.0
+Tecan.At.XFluor.Device.AMRPlus, 1.9.17.0
+Tecan.At.XFluor.Device.GeniosUltra, 1.9.17.0
+Tecan.At.XFluor.Device.Reader, 1.9.17.0
+Tecan.At.XFluor.Device.Safire3, 1.9.17.0
+Tecan.At.XFluor.Device.Safire3Pro, 1.9.17.0
+Tecan.At.XFluor.Device.SunriseMini, 1.9.17.0
+Tecan.At.XFluor.ExcelOutput, 1.9.17.0
+Tecan.At.XFluor.NanoQuant, 1.9.17.0
+Tecan.At.XFluor.ReaderEditor, 1.9.17.0
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">MEX, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
+MEM, V 1.20 Safire2 MCR  (V 1.20 Safire2 MCR )
+ABS, V 1.00 MCR Abs 4 Channel (V 1.00 MCR Abs 4 Channel)
+LUM, V_1.04_11/2011_LUMINESCENCE (Nov 02 2011/17.53.34)
+TCAN, V_1.00_02/2008_S3FTCAN (Feb 21 2008/17.19.16)
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="73">
   <si>
     <t>Application: Tecan i-control</t>
   </si>
@@ -668,6 +933,33 @@
   </si>
   <si>
     <t>H</t>
+  </si>
+  <si>
+    <t>10:35:22 AM</t>
+  </si>
+  <si>
+    <t>FHCRC\reguia</t>
+  </si>
+  <si>
+    <t>5/23/2019 10:36:17 AM</t>
+  </si>
+  <si>
+    <t>Temperature: 24.7 °C</t>
+  </si>
+  <si>
+    <t>5/23/2019 10:37:13 AM</t>
+  </si>
+  <si>
+    <t>10:37:35 AM</t>
+  </si>
+  <si>
+    <t>5/23/2019 10:38:38 AM</t>
+  </si>
+  <si>
+    <t>Temperature: 25 °C</t>
+  </si>
+  <si>
+    <t>5/23/2019 10:39:34 AM</t>
   </si>
 </sst>
 </file>
@@ -847,7 +1139,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -882,7 +1174,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -1093,13 +1385,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1107,7 +1399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1115,7 +1407,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1123,7 +1415,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1131,7 +1423,7 @@
         <v>43580</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1139,7 +1431,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1147,7 +1439,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1155,7 +1447,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1163,17 +1455,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1181,12 +1473,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13">
       <c r="A17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -1197,7 +1489,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -1208,7 +1500,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -1219,7 +1511,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -1230,7 +1522,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -1241,7 +1533,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -1252,7 +1544,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -1263,7 +1555,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -1274,7 +1566,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -1285,7 +1577,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -1296,7 +1588,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -1304,12 +1596,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13">
       <c r="B30" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13">
       <c r="A31" s="3" t="s">
         <v>39</v>
       </c>
@@ -1350,12 +1642,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13">
       <c r="A32" s="3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13">
       <c r="A33" s="3" t="s">
         <v>40</v>
       </c>
@@ -1396,7 +1688,7 @@
         <v>19083</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13">
       <c r="A34" s="3" t="s">
         <v>41</v>
       </c>
@@ -1437,7 +1729,7 @@
         <v>35752</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13">
       <c r="A35" s="3" t="s">
         <v>42</v>
       </c>
@@ -1478,7 +1770,7 @@
         <v>23617</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13">
       <c r="A36" s="3" t="s">
         <v>43</v>
       </c>
@@ -1519,7 +1811,7 @@
         <v>25105</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13">
       <c r="A37" s="3" t="s">
         <v>44</v>
       </c>
@@ -1560,7 +1852,7 @@
         <v>25178</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13">
       <c r="A38" s="3" t="s">
         <v>45</v>
       </c>
@@ -1601,12 +1893,12 @@
         <v>34660</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13">
       <c r="A39" s="3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13">
       <c r="A42" t="s">
         <v>46</v>
       </c>
@@ -1617,6 +1909,11 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1628,9 +1925,9 @@
       <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1638,7 +1935,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1646,7 +1943,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1654,7 +1951,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1662,7 +1959,7 @@
         <v>43580</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1670,7 +1967,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1678,7 +1975,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1686,7 +1983,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1694,17 +1991,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1712,12 +2009,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13">
       <c r="A17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -1728,7 +2025,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -1739,7 +2036,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -1750,7 +2047,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -1761,7 +2058,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -1772,7 +2069,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -1783,7 +2080,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -1794,7 +2091,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -1805,7 +2102,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -1816,7 +2113,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -1827,7 +2124,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -1835,12 +2132,12 @@
         <v>49</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13">
       <c r="B30" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13">
       <c r="A31" s="3" t="s">
         <v>39</v>
       </c>
@@ -1881,12 +2178,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13">
       <c r="A32" s="3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13">
       <c r="A33" s="3" t="s">
         <v>40</v>
       </c>
@@ -1927,7 +2224,7 @@
         <v>10317</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13">
       <c r="A34" s="3" t="s">
         <v>41</v>
       </c>
@@ -1968,7 +2265,7 @@
         <v>26800</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13">
       <c r="A35" s="3" t="s">
         <v>42</v>
       </c>
@@ -2009,7 +2306,7 @@
         <v>19118</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13">
       <c r="A36" s="3" t="s">
         <v>43</v>
       </c>
@@ -2050,7 +2347,7 @@
         <v>18910</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13">
       <c r="A37" s="3" t="s">
         <v>44</v>
       </c>
@@ -2091,7 +2388,7 @@
         <v>18630</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13">
       <c r="A38" s="3" t="s">
         <v>45</v>
       </c>
@@ -2132,12 +2429,12 @@
         <v>25472</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13">
       <c r="A39" s="3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13">
       <c r="A42" t="s">
         <v>46</v>
       </c>
@@ -2148,6 +2445,11 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2159,9 +2461,9 @@
       <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2169,7 +2471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2177,7 +2479,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2185,7 +2487,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -2193,7 +2495,7 @@
         <v>43580</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -2201,7 +2503,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -2209,7 +2511,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -2217,7 +2519,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -2225,17 +2527,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -2243,12 +2545,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13">
       <c r="A17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -2259,7 +2561,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -2270,7 +2572,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -2281,7 +2583,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -2292,7 +2594,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -2303,7 +2605,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -2314,7 +2616,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -2325,7 +2627,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -2336,7 +2638,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -2347,7 +2649,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -2358,7 +2660,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -2366,12 +2668,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13">
       <c r="B30" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13">
       <c r="A31" s="3" t="s">
         <v>39</v>
       </c>
@@ -2412,12 +2714,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13">
       <c r="A32" s="3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13">
       <c r="A33" s="3" t="s">
         <v>40</v>
       </c>
@@ -2458,7 +2760,7 @@
         <v>11992</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13">
       <c r="A34" s="3" t="s">
         <v>41</v>
       </c>
@@ -2499,7 +2801,7 @@
         <v>32498</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13">
       <c r="A35" s="3" t="s">
         <v>42</v>
       </c>
@@ -2540,7 +2842,7 @@
         <v>15846</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13">
       <c r="A36" s="3" t="s">
         <v>43</v>
       </c>
@@ -2581,7 +2883,7 @@
         <v>16944</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13">
       <c r="A37" s="3" t="s">
         <v>44</v>
       </c>
@@ -2622,7 +2924,7 @@
         <v>17995</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13">
       <c r="A38" s="3" t="s">
         <v>45</v>
       </c>
@@ -2663,12 +2965,12 @@
         <v>29897</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13">
       <c r="A39" s="3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13">
       <c r="A42" t="s">
         <v>46</v>
       </c>
@@ -2679,6 +2981,11 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2690,9 +2997,9 @@
       <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2700,7 +3007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2708,7 +3015,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2716,7 +3023,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -2724,7 +3031,7 @@
         <v>43580</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -2732,7 +3039,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -2740,7 +3047,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -2748,7 +3055,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -2756,17 +3063,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -2774,12 +3081,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13">
       <c r="A17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -2790,7 +3097,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -2801,7 +3108,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -2812,7 +3119,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -2823,7 +3130,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -2834,7 +3141,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -2845,7 +3152,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -2856,7 +3163,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -2867,7 +3174,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -2878,7 +3185,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -2889,7 +3196,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -2897,12 +3204,12 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13">
       <c r="B30" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13">
       <c r="A31" s="3" t="s">
         <v>39</v>
       </c>
@@ -2943,12 +3250,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13">
       <c r="A32" s="3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13">
       <c r="A33" s="3" t="s">
         <v>40</v>
       </c>
@@ -2989,7 +3296,7 @@
         <v>11351</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13">
       <c r="A34" s="3" t="s">
         <v>41</v>
       </c>
@@ -3030,7 +3337,7 @@
         <v>31318</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13">
       <c r="A35" s="3" t="s">
         <v>42</v>
       </c>
@@ -3071,7 +3378,7 @@
         <v>17667</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13">
       <c r="A36" s="3" t="s">
         <v>43</v>
       </c>
@@ -3112,7 +3419,7 @@
         <v>17756</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13">
       <c r="A37" s="3" t="s">
         <v>44</v>
       </c>
@@ -3153,7 +3460,7 @@
         <v>17781</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13">
       <c r="A38" s="3" t="s">
         <v>45</v>
       </c>
@@ -3194,12 +3501,12 @@
         <v>30179</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13">
       <c r="A39" s="3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13">
       <c r="A42" t="s">
         <v>46</v>
       </c>
@@ -3210,6 +3517,11 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3221,9 +3533,9 @@
       <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3231,7 +3543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -3239,7 +3551,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -3247,7 +3559,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -3255,7 +3567,7 @@
         <v>43580</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -3263,7 +3575,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -3271,7 +3583,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -3279,7 +3591,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -3287,17 +3599,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -3305,12 +3617,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13">
       <c r="A17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -3321,7 +3633,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -3332,7 +3644,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -3343,7 +3655,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -3354,7 +3666,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -3365,7 +3677,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -3376,7 +3688,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -3387,7 +3699,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -3398,7 +3710,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -3409,7 +3721,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -3420,7 +3732,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -3428,12 +3740,12 @@
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13">
       <c r="B30" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13">
       <c r="A31" s="3" t="s">
         <v>39</v>
       </c>
@@ -3474,12 +3786,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13">
       <c r="A32" s="3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13">
       <c r="A33" s="3" t="s">
         <v>40</v>
       </c>
@@ -3520,7 +3832,7 @@
         <v>6063</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13">
       <c r="A34" s="3" t="s">
         <v>41</v>
       </c>
@@ -3561,7 +3873,7 @@
         <v>16688</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13">
       <c r="A35" s="3" t="s">
         <v>42</v>
       </c>
@@ -3602,7 +3914,7 @@
         <v>7945</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13">
       <c r="A36" s="3" t="s">
         <v>43</v>
       </c>
@@ -3643,7 +3955,7 @@
         <v>8141</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13">
       <c r="A37" s="3" t="s">
         <v>44</v>
       </c>
@@ -3684,7 +3996,7 @@
         <v>8289</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13">
       <c r="A38" s="3" t="s">
         <v>45</v>
       </c>
@@ -3725,12 +4037,12 @@
         <v>14122</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13">
       <c r="A39" s="3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13">
       <c r="A42" t="s">
         <v>46</v>
       </c>
@@ -3741,5 +4053,1834 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M43"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L37" sqref="L37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1">
+        <v>43608</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18">
+        <v>485</v>
+      </c>
+      <c r="F18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19">
+        <v>515</v>
+      </c>
+      <c r="F19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20">
+        <v>12</v>
+      </c>
+      <c r="F20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21">
+        <v>12</v>
+      </c>
+      <c r="F21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22">
+        <v>108</v>
+      </c>
+      <c r="F22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23">
+        <v>25</v>
+      </c>
+      <c r="F23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+      <c r="E24">
+        <v>400</v>
+      </c>
+      <c r="F24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25" t="s">
+        <v>31</v>
+      </c>
+      <c r="E25">
+        <v>20</v>
+      </c>
+      <c r="F25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="A27" t="s">
+        <v>34</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="A28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="B30" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="A31" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" s="3">
+        <v>1</v>
+      </c>
+      <c r="C31" s="3">
+        <v>2</v>
+      </c>
+      <c r="D31" s="3">
+        <v>3</v>
+      </c>
+      <c r="E31" s="3">
+        <v>4</v>
+      </c>
+      <c r="F31" s="3">
+        <v>5</v>
+      </c>
+      <c r="G31" s="3">
+        <v>6</v>
+      </c>
+      <c r="H31" s="3">
+        <v>7</v>
+      </c>
+      <c r="I31" s="3">
+        <v>8</v>
+      </c>
+      <c r="J31" s="3">
+        <v>9</v>
+      </c>
+      <c r="K31" s="3">
+        <v>10</v>
+      </c>
+      <c r="L31" s="3">
+        <v>11</v>
+      </c>
+      <c r="M31" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="A32" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32">
+        <v>13425</v>
+      </c>
+      <c r="C32">
+        <v>13878</v>
+      </c>
+      <c r="D32">
+        <v>14012</v>
+      </c>
+      <c r="E32">
+        <v>14302</v>
+      </c>
+      <c r="F32">
+        <v>15037</v>
+      </c>
+      <c r="G32">
+        <v>15029</v>
+      </c>
+      <c r="H32">
+        <v>14734</v>
+      </c>
+      <c r="I32">
+        <v>14554</v>
+      </c>
+      <c r="J32">
+        <v>14438</v>
+      </c>
+      <c r="K32">
+        <v>14280</v>
+      </c>
+      <c r="L32">
+        <v>13889</v>
+      </c>
+      <c r="M32">
+        <v>13150</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13">
+      <c r="A33" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33">
+        <v>19799</v>
+      </c>
+      <c r="C33">
+        <v>20322</v>
+      </c>
+      <c r="D33">
+        <v>20411</v>
+      </c>
+      <c r="E33">
+        <v>20416</v>
+      </c>
+      <c r="F33">
+        <v>20696</v>
+      </c>
+      <c r="G33">
+        <v>21009</v>
+      </c>
+      <c r="H33">
+        <v>20568</v>
+      </c>
+      <c r="I33">
+        <v>20545</v>
+      </c>
+      <c r="J33">
+        <v>20590</v>
+      </c>
+      <c r="K33">
+        <v>20309</v>
+      </c>
+      <c r="L33">
+        <v>20237</v>
+      </c>
+      <c r="M33">
+        <v>19864</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13">
+      <c r="A34" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34">
+        <v>32716</v>
+      </c>
+      <c r="C34">
+        <v>32155</v>
+      </c>
+      <c r="D34">
+        <v>36329</v>
+      </c>
+      <c r="E34">
+        <v>34641</v>
+      </c>
+      <c r="F34">
+        <v>36225</v>
+      </c>
+      <c r="G34">
+        <v>36695</v>
+      </c>
+      <c r="H34">
+        <v>36579</v>
+      </c>
+      <c r="I34">
+        <v>36711</v>
+      </c>
+      <c r="J34">
+        <v>36628</v>
+      </c>
+      <c r="K34">
+        <v>35841</v>
+      </c>
+      <c r="L34">
+        <v>36422</v>
+      </c>
+      <c r="M34">
+        <v>33568</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
+      <c r="A35" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B35">
+        <v>33806</v>
+      </c>
+      <c r="C35">
+        <v>34099</v>
+      </c>
+      <c r="D35">
+        <v>35623</v>
+      </c>
+      <c r="E35">
+        <v>35850</v>
+      </c>
+      <c r="F35">
+        <v>36613</v>
+      </c>
+      <c r="G35">
+        <v>34332</v>
+      </c>
+      <c r="H35">
+        <v>32259</v>
+      </c>
+      <c r="I35">
+        <v>24664</v>
+      </c>
+      <c r="J35">
+        <v>22046</v>
+      </c>
+      <c r="K35">
+        <v>22364</v>
+      </c>
+      <c r="L35">
+        <v>24253</v>
+      </c>
+      <c r="M35">
+        <v>28720</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13">
+      <c r="A36" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B36">
+        <v>31874</v>
+      </c>
+      <c r="C36">
+        <v>33378</v>
+      </c>
+      <c r="D36">
+        <v>34413</v>
+      </c>
+      <c r="E36">
+        <v>36898</v>
+      </c>
+      <c r="F36">
+        <v>36654</v>
+      </c>
+      <c r="G36">
+        <v>34812</v>
+      </c>
+      <c r="H36">
+        <v>29294</v>
+      </c>
+      <c r="I36">
+        <v>24807</v>
+      </c>
+      <c r="J36">
+        <v>22015</v>
+      </c>
+      <c r="K36">
+        <v>22091</v>
+      </c>
+      <c r="L36">
+        <v>24725</v>
+      </c>
+      <c r="M36">
+        <v>28829</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="A37" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37">
+        <v>32518</v>
+      </c>
+      <c r="C37">
+        <v>32483</v>
+      </c>
+      <c r="D37">
+        <v>33084</v>
+      </c>
+      <c r="E37">
+        <v>34428</v>
+      </c>
+      <c r="F37">
+        <v>35154</v>
+      </c>
+      <c r="G37">
+        <v>31975</v>
+      </c>
+      <c r="H37">
+        <v>31652</v>
+      </c>
+      <c r="I37">
+        <v>25143</v>
+      </c>
+      <c r="J37">
+        <v>21692</v>
+      </c>
+      <c r="K37">
+        <v>22150</v>
+      </c>
+      <c r="L37">
+        <v>25038</v>
+      </c>
+      <c r="M37">
+        <v>28852</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
+      <c r="A38" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38">
+        <v>32206</v>
+      </c>
+      <c r="C38">
+        <v>31673</v>
+      </c>
+      <c r="D38">
+        <v>32222</v>
+      </c>
+      <c r="E38">
+        <v>32619</v>
+      </c>
+      <c r="F38">
+        <v>32410</v>
+      </c>
+      <c r="G38">
+        <v>34095</v>
+      </c>
+      <c r="H38">
+        <v>36718</v>
+      </c>
+      <c r="I38">
+        <v>33771</v>
+      </c>
+      <c r="J38">
+        <v>36056</v>
+      </c>
+      <c r="K38">
+        <v>33274</v>
+      </c>
+      <c r="L38">
+        <v>33590</v>
+      </c>
+      <c r="M38">
+        <v>33151</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13">
+      <c r="A39" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B39">
+        <v>12866</v>
+      </c>
+      <c r="C39">
+        <v>13593</v>
+      </c>
+      <c r="D39">
+        <v>13186</v>
+      </c>
+      <c r="E39">
+        <v>13630</v>
+      </c>
+      <c r="F39">
+        <v>13843</v>
+      </c>
+      <c r="G39">
+        <v>13991</v>
+      </c>
+      <c r="H39">
+        <v>13903</v>
+      </c>
+      <c r="I39">
+        <v>13742</v>
+      </c>
+      <c r="J39">
+        <v>13597</v>
+      </c>
+      <c r="K39">
+        <v>13332</v>
+      </c>
+      <c r="L39">
+        <v>12901</v>
+      </c>
+      <c r="M39">
+        <v>12521</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13">
+      <c r="A43" t="s">
+        <v>46</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M43"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1">
+        <v>43608</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18">
+        <v>485</v>
+      </c>
+      <c r="F18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19">
+        <v>515</v>
+      </c>
+      <c r="F19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20">
+        <v>12</v>
+      </c>
+      <c r="F20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21">
+        <v>12</v>
+      </c>
+      <c r="F21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22">
+        <v>108</v>
+      </c>
+      <c r="F22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23">
+        <v>25</v>
+      </c>
+      <c r="F23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+      <c r="E24">
+        <v>400</v>
+      </c>
+      <c r="F24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25" t="s">
+        <v>31</v>
+      </c>
+      <c r="E25">
+        <v>20</v>
+      </c>
+      <c r="F25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="A27" t="s">
+        <v>34</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="A28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="B30" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="A31" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" s="3">
+        <v>1</v>
+      </c>
+      <c r="C31" s="3">
+        <v>2</v>
+      </c>
+      <c r="D31" s="3">
+        <v>3</v>
+      </c>
+      <c r="E31" s="3">
+        <v>4</v>
+      </c>
+      <c r="F31" s="3">
+        <v>5</v>
+      </c>
+      <c r="G31" s="3">
+        <v>6</v>
+      </c>
+      <c r="H31" s="3">
+        <v>7</v>
+      </c>
+      <c r="I31" s="3">
+        <v>8</v>
+      </c>
+      <c r="J31" s="3">
+        <v>9</v>
+      </c>
+      <c r="K31" s="3">
+        <v>10</v>
+      </c>
+      <c r="L31" s="3">
+        <v>11</v>
+      </c>
+      <c r="M31" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="A32" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32">
+        <v>13425</v>
+      </c>
+      <c r="C32">
+        <v>13878</v>
+      </c>
+      <c r="D32">
+        <v>14012</v>
+      </c>
+      <c r="E32">
+        <v>14302</v>
+      </c>
+      <c r="F32">
+        <v>15037</v>
+      </c>
+      <c r="G32">
+        <v>15029</v>
+      </c>
+      <c r="H32">
+        <v>14734</v>
+      </c>
+      <c r="I32">
+        <v>14554</v>
+      </c>
+      <c r="J32">
+        <v>14438</v>
+      </c>
+      <c r="K32">
+        <v>14280</v>
+      </c>
+      <c r="L32">
+        <v>13889</v>
+      </c>
+      <c r="M32">
+        <v>13150</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13">
+      <c r="A33" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33">
+        <v>19799</v>
+      </c>
+      <c r="C33">
+        <v>20322</v>
+      </c>
+      <c r="D33">
+        <v>20411</v>
+      </c>
+      <c r="E33">
+        <v>20416</v>
+      </c>
+      <c r="F33">
+        <v>20696</v>
+      </c>
+      <c r="G33">
+        <v>21009</v>
+      </c>
+      <c r="H33">
+        <v>20568</v>
+      </c>
+      <c r="I33">
+        <v>20545</v>
+      </c>
+      <c r="J33">
+        <v>20590</v>
+      </c>
+      <c r="K33">
+        <v>20309</v>
+      </c>
+      <c r="L33">
+        <v>20237</v>
+      </c>
+      <c r="M33">
+        <v>19864</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13">
+      <c r="A34" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34">
+        <v>32716</v>
+      </c>
+      <c r="C34">
+        <v>32155</v>
+      </c>
+      <c r="D34">
+        <v>36329</v>
+      </c>
+      <c r="E34">
+        <v>34641</v>
+      </c>
+      <c r="F34">
+        <v>36225</v>
+      </c>
+      <c r="G34">
+        <v>36695</v>
+      </c>
+      <c r="H34">
+        <v>36579</v>
+      </c>
+      <c r="I34">
+        <v>36711</v>
+      </c>
+      <c r="J34">
+        <v>36628</v>
+      </c>
+      <c r="K34">
+        <v>35841</v>
+      </c>
+      <c r="L34">
+        <v>36422</v>
+      </c>
+      <c r="M34">
+        <v>33568</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
+      <c r="A35" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B35">
+        <v>33806</v>
+      </c>
+      <c r="C35">
+        <v>34099</v>
+      </c>
+      <c r="D35">
+        <v>35623</v>
+      </c>
+      <c r="E35">
+        <v>35850</v>
+      </c>
+      <c r="F35">
+        <v>36613</v>
+      </c>
+      <c r="G35">
+        <v>34332</v>
+      </c>
+      <c r="H35">
+        <v>32259</v>
+      </c>
+      <c r="I35">
+        <v>24664</v>
+      </c>
+      <c r="J35">
+        <v>22046</v>
+      </c>
+      <c r="K35">
+        <v>22364</v>
+      </c>
+      <c r="L35">
+        <v>24253</v>
+      </c>
+      <c r="M35">
+        <v>28720</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13">
+      <c r="A36" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B36">
+        <v>31874</v>
+      </c>
+      <c r="C36">
+        <v>33378</v>
+      </c>
+      <c r="D36">
+        <v>34413</v>
+      </c>
+      <c r="E36">
+        <v>36898</v>
+      </c>
+      <c r="F36">
+        <v>36654</v>
+      </c>
+      <c r="G36">
+        <v>34812</v>
+      </c>
+      <c r="H36">
+        <v>29294</v>
+      </c>
+      <c r="I36">
+        <v>24807</v>
+      </c>
+      <c r="J36">
+        <v>22015</v>
+      </c>
+      <c r="K36">
+        <v>22091</v>
+      </c>
+      <c r="L36">
+        <v>24725</v>
+      </c>
+      <c r="M36">
+        <v>28829</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="A37" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37">
+        <v>32518</v>
+      </c>
+      <c r="C37">
+        <v>32483</v>
+      </c>
+      <c r="D37">
+        <v>33084</v>
+      </c>
+      <c r="E37">
+        <v>34428</v>
+      </c>
+      <c r="F37">
+        <v>35154</v>
+      </c>
+      <c r="G37">
+        <v>31975</v>
+      </c>
+      <c r="H37">
+        <v>31652</v>
+      </c>
+      <c r="I37">
+        <v>25143</v>
+      </c>
+      <c r="J37">
+        <v>21692</v>
+      </c>
+      <c r="K37">
+        <v>22150</v>
+      </c>
+      <c r="L37">
+        <v>25038</v>
+      </c>
+      <c r="M37">
+        <v>28852</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
+      <c r="A38" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38">
+        <v>32206</v>
+      </c>
+      <c r="C38">
+        <v>31673</v>
+      </c>
+      <c r="D38">
+        <v>32222</v>
+      </c>
+      <c r="E38">
+        <v>32619</v>
+      </c>
+      <c r="F38">
+        <v>32410</v>
+      </c>
+      <c r="G38">
+        <v>34095</v>
+      </c>
+      <c r="H38">
+        <v>36718</v>
+      </c>
+      <c r="I38">
+        <v>33771</v>
+      </c>
+      <c r="J38">
+        <v>36056</v>
+      </c>
+      <c r="K38">
+        <v>33274</v>
+      </c>
+      <c r="L38">
+        <v>33590</v>
+      </c>
+      <c r="M38">
+        <v>33151</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13">
+      <c r="A39" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B39">
+        <v>12866</v>
+      </c>
+      <c r="C39">
+        <v>13593</v>
+      </c>
+      <c r="D39">
+        <v>13186</v>
+      </c>
+      <c r="E39">
+        <v>13630</v>
+      </c>
+      <c r="F39">
+        <v>13843</v>
+      </c>
+      <c r="G39">
+        <v>13991</v>
+      </c>
+      <c r="H39">
+        <v>13903</v>
+      </c>
+      <c r="I39">
+        <v>13742</v>
+      </c>
+      <c r="J39">
+        <v>13597</v>
+      </c>
+      <c r="K39">
+        <v>13332</v>
+      </c>
+      <c r="L39">
+        <v>12901</v>
+      </c>
+      <c r="M39">
+        <v>12521</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13">
+      <c r="A43" t="s">
+        <v>46</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1">
+        <v>43608</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18">
+        <v>485</v>
+      </c>
+      <c r="F18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19">
+        <v>515</v>
+      </c>
+      <c r="F19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20">
+        <v>12</v>
+      </c>
+      <c r="F20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21">
+        <v>12</v>
+      </c>
+      <c r="F21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22">
+        <v>97</v>
+      </c>
+      <c r="F22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23">
+        <v>25</v>
+      </c>
+      <c r="F23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+      <c r="E24">
+        <v>400</v>
+      </c>
+      <c r="F24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25" t="s">
+        <v>31</v>
+      </c>
+      <c r="E25">
+        <v>20</v>
+      </c>
+      <c r="F25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="A27" t="s">
+        <v>34</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="A28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="B30" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="A31" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" s="3">
+        <v>1</v>
+      </c>
+      <c r="C31" s="3">
+        <v>2</v>
+      </c>
+      <c r="D31" s="3">
+        <v>3</v>
+      </c>
+      <c r="E31" s="3">
+        <v>4</v>
+      </c>
+      <c r="F31" s="3">
+        <v>5</v>
+      </c>
+      <c r="G31" s="3">
+        <v>6</v>
+      </c>
+      <c r="H31" s="3">
+        <v>7</v>
+      </c>
+      <c r="I31" s="3">
+        <v>8</v>
+      </c>
+      <c r="J31" s="3">
+        <v>9</v>
+      </c>
+      <c r="K31" s="3">
+        <v>10</v>
+      </c>
+      <c r="L31" s="3">
+        <v>11</v>
+      </c>
+      <c r="M31" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="A32" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32">
+        <v>6206</v>
+      </c>
+      <c r="C32">
+        <v>6347</v>
+      </c>
+      <c r="D32">
+        <v>6756</v>
+      </c>
+      <c r="E32">
+        <v>6866</v>
+      </c>
+      <c r="F32">
+        <v>6946</v>
+      </c>
+      <c r="G32">
+        <v>6936</v>
+      </c>
+      <c r="H32">
+        <v>6977</v>
+      </c>
+      <c r="I32">
+        <v>6674</v>
+      </c>
+      <c r="J32">
+        <v>6968</v>
+      </c>
+      <c r="K32">
+        <v>6551</v>
+      </c>
+      <c r="L32">
+        <v>6424</v>
+      </c>
+      <c r="M32">
+        <v>6206</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13">
+      <c r="A33" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33">
+        <v>9880</v>
+      </c>
+      <c r="C33">
+        <v>9919</v>
+      </c>
+      <c r="D33">
+        <v>9980</v>
+      </c>
+      <c r="E33">
+        <v>10048</v>
+      </c>
+      <c r="F33">
+        <v>10269</v>
+      </c>
+      <c r="G33">
+        <v>10276</v>
+      </c>
+      <c r="H33">
+        <v>10058</v>
+      </c>
+      <c r="I33">
+        <v>10138</v>
+      </c>
+      <c r="J33">
+        <v>10151</v>
+      </c>
+      <c r="K33">
+        <v>10102</v>
+      </c>
+      <c r="L33">
+        <v>9804</v>
+      </c>
+      <c r="M33">
+        <v>9757</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13">
+      <c r="A34" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34">
+        <v>28369</v>
+      </c>
+      <c r="C34">
+        <v>33664</v>
+      </c>
+      <c r="D34">
+        <v>34571</v>
+      </c>
+      <c r="E34">
+        <v>34633</v>
+      </c>
+      <c r="F34">
+        <v>36268</v>
+      </c>
+      <c r="G34">
+        <v>36563</v>
+      </c>
+      <c r="H34">
+        <v>36473</v>
+      </c>
+      <c r="I34">
+        <v>35113</v>
+      </c>
+      <c r="J34">
+        <v>36206</v>
+      </c>
+      <c r="K34">
+        <v>34983</v>
+      </c>
+      <c r="L34">
+        <v>32721</v>
+      </c>
+      <c r="M34">
+        <v>28945</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
+      <c r="A35" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B35">
+        <v>25866</v>
+      </c>
+      <c r="C35">
+        <v>31357</v>
+      </c>
+      <c r="D35">
+        <v>33150</v>
+      </c>
+      <c r="E35">
+        <v>35289</v>
+      </c>
+      <c r="F35">
+        <v>35131</v>
+      </c>
+      <c r="G35">
+        <v>33582</v>
+      </c>
+      <c r="H35">
+        <v>34609</v>
+      </c>
+      <c r="I35">
+        <v>26976</v>
+      </c>
+      <c r="J35">
+        <v>20609</v>
+      </c>
+      <c r="K35">
+        <v>12394</v>
+      </c>
+      <c r="L35">
+        <v>12133</v>
+      </c>
+      <c r="M35">
+        <v>13834</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13">
+      <c r="A36" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B36">
+        <v>27370</v>
+      </c>
+      <c r="C36">
+        <v>32189</v>
+      </c>
+      <c r="D36">
+        <v>32684</v>
+      </c>
+      <c r="E36">
+        <v>35130</v>
+      </c>
+      <c r="F36">
+        <v>36068</v>
+      </c>
+      <c r="G36">
+        <v>34002</v>
+      </c>
+      <c r="H36">
+        <v>33182</v>
+      </c>
+      <c r="I36">
+        <v>27563</v>
+      </c>
+      <c r="J36">
+        <v>19692</v>
+      </c>
+      <c r="K36">
+        <v>12350</v>
+      </c>
+      <c r="L36">
+        <v>11938</v>
+      </c>
+      <c r="M36">
+        <v>14006</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="A37" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37">
+        <v>27614</v>
+      </c>
+      <c r="C37">
+        <v>32150</v>
+      </c>
+      <c r="D37">
+        <v>33210</v>
+      </c>
+      <c r="E37">
+        <v>32878</v>
+      </c>
+      <c r="F37">
+        <v>36283</v>
+      </c>
+      <c r="G37">
+        <v>32246</v>
+      </c>
+      <c r="H37">
+        <v>32580</v>
+      </c>
+      <c r="I37">
+        <v>28265</v>
+      </c>
+      <c r="J37">
+        <v>18229</v>
+      </c>
+      <c r="K37">
+        <v>11951</v>
+      </c>
+      <c r="L37">
+        <v>11841</v>
+      </c>
+      <c r="M37">
+        <v>13868</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
+      <c r="A38" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38">
+        <v>30239</v>
+      </c>
+      <c r="C38">
+        <v>28654</v>
+      </c>
+      <c r="D38">
+        <v>30585</v>
+      </c>
+      <c r="E38">
+        <v>29802</v>
+      </c>
+      <c r="F38">
+        <v>32657</v>
+      </c>
+      <c r="G38">
+        <v>30893</v>
+      </c>
+      <c r="H38">
+        <v>31064</v>
+      </c>
+      <c r="I38">
+        <v>32461</v>
+      </c>
+      <c r="J38">
+        <v>31293</v>
+      </c>
+      <c r="K38">
+        <v>29848</v>
+      </c>
+      <c r="L38">
+        <v>29485</v>
+      </c>
+      <c r="M38">
+        <v>26422</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13">
+      <c r="A39" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B39">
+        <v>5930</v>
+      </c>
+      <c r="C39">
+        <v>6037</v>
+      </c>
+      <c r="D39">
+        <v>6245</v>
+      </c>
+      <c r="E39">
+        <v>6368</v>
+      </c>
+      <c r="F39">
+        <v>6474</v>
+      </c>
+      <c r="G39">
+        <v>6550</v>
+      </c>
+      <c r="H39">
+        <v>6464</v>
+      </c>
+      <c r="I39">
+        <v>6460</v>
+      </c>
+      <c r="J39">
+        <v>6390</v>
+      </c>
+      <c r="K39">
+        <v>6284</v>
+      </c>
+      <c r="L39">
+        <v>5961</v>
+      </c>
+      <c r="M39">
+        <v>5730</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13">
+      <c r="A43" t="s">
+        <v>46</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>